<commit_message>
Primi tentativi di riduzione
</commit_message>
<xml_diff>
--- a/pagine tesi.xlsx
+++ b/pagine tesi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saint\newtesi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\newtesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299030A9-51ED-4FF9-B2D7-B0A50FCE667D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB792C0-F535-4190-B4DA-2E1BC0628734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{219FEE24-269F-49AC-ADBB-AC69005E8BC9}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">cap1 </t>
   </si>
@@ -47,9 +36,6 @@
     <t>cap2</t>
   </si>
   <si>
-    <t>cp2rev</t>
-  </si>
-  <si>
     <t>cap3</t>
   </si>
   <si>
@@ -72,13 +58,34 @@
   </si>
   <si>
     <t>Rev</t>
+  </si>
+  <si>
+    <t>cap1 final</t>
+  </si>
+  <si>
+    <t>cap2rev</t>
+  </si>
+  <si>
+    <t>cap2 final</t>
+  </si>
+  <si>
+    <t>cap3 final</t>
+  </si>
+  <si>
+    <t>cap4 final</t>
+  </si>
+  <si>
+    <t>cap5 final</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,7 +474,7 @@
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
-      <we:customFunctionIdList>
+      <we:customFunctionIdList xmlns="">
         <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_GPT_LIST</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_GPT_HLIST</we:customFunctionIds>
@@ -494,15 +501,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9035CA-6349-41F5-B5D9-3539DACE0FC0}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,11 +527,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <f>B1+1</f>
         <v>2</v>
       </c>
       <c r="C2">
@@ -534,172 +542,282 @@
         <v>31</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F10" si="0">D2-C2</f>
+        <f t="shared" ref="F2:F15" si="0">D2-C2</f>
         <v>5</v>
       </c>
       <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3">
+        <f t="shared" ref="B3:B15" si="1">B2+1</f>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>55</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <f>F1+F4+F7+F10+F13</f>
+        <v>93</v>
+      </c>
+      <c r="J4">
+        <f>F2+F5+F8+F11+F14</f>
+        <v>72</v>
+      </c>
+      <c r="K4">
+        <f>F3+F6+F9+F12+F15</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>33</v>
-      </c>
-      <c r="D3">
-        <v>55</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="I3">
-        <f>F1+F3+F5+F7+F9</f>
-        <v>93</v>
-      </c>
-      <c r="J3">
-        <f>F12-I3</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>98</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>57</v>
-      </c>
-      <c r="D4">
-        <v>72</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>117</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>113</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>120</v>
+      </c>
+      <c r="D10">
+        <v>134</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>136</v>
+      </c>
+      <c r="D11">
+        <v>156</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>75</v>
-      </c>
-      <c r="D5">
-        <v>98</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>117</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>116</v>
+      </c>
+      <c r="D12">
+        <v>172</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>120</v>
-      </c>
-      <c r="D7">
-        <v>134</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>158</v>
+      </c>
+      <c r="D13">
+        <v>170</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>136</v>
-      </c>
-      <c r="D8">
-        <v>156</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>158</v>
-      </c>
-      <c r="D9">
-        <v>170</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10">
+      <c r="C14">
         <v>172</v>
       </c>
-      <c r="D10">
+      <c r="D14">
         <v>187</v>
       </c>
-      <c r="F10">
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f>SUM(F1:F11)</f>
-        <v>165</v>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>175</v>
+      </c>
+      <c r="D15">
+        <v>193</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17">
+        <f>SUM(F1:F16)</f>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>